<commit_message>
update to add additional test data (part 1)
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Fall2023/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F283CED0-1CA2-4959-95F5-034E429376AB}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907EC92E-6BDA-4D08-A3AC-0F3A6EDB9D27}"/>
   <bookViews>
-    <workbookView xWindow="-36840" yWindow="690" windowWidth="19815" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24495" yWindow="1650" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Test</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>VaR/ES on 2 levels from simulated values</t>
+  </si>
+  <si>
+    <t>test7_1.csv</t>
+  </si>
+  <si>
+    <t>test7_2.csv</t>
+  </si>
+  <si>
+    <t>test7_3.csv</t>
   </si>
 </sst>
 </file>
@@ -490,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,6 +815,9 @@
       <c r="B21" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>testout_7.1.csv</v>
@@ -818,6 +830,9 @@
       <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>testout_7.2.csv</v>
@@ -829,6 +844,9 @@
       </c>
       <c r="B23" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
updates for tests part 2
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Fall2023/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907EC92E-6BDA-4D08-A3AC-0F3A6EDB9D27}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67110BD-B845-4D63-BBDC-92D93476919A}"/>
   <bookViews>
-    <workbookView xWindow="-24495" yWindow="1650" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25560" yWindow="1560" windowWidth="21735" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Test</t>
   </si>
@@ -149,18 +149,12 @@
     <t>Var from T Distribution</t>
   </si>
   <si>
-    <t>VaR from Simulation</t>
-  </si>
-  <si>
     <t>ES From Normal Distribution</t>
   </si>
   <si>
     <t>ES from T Distribution</t>
   </si>
   <si>
-    <t>ES from Simulation</t>
-  </si>
-  <si>
     <t>Gaussian Copula with a  Normal and T distribution</t>
   </si>
   <si>
@@ -177,6 +171,12 @@
   </si>
   <si>
     <t>test7_3.csv</t>
+  </si>
+  <si>
+    <t>VaR from Simulation -- compare to 8.2 values</t>
+  </si>
+  <si>
+    <t>ES from Simulation -- compare to 8.5 values</t>
   </si>
 </sst>
 </file>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +816,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -831,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -846,7 +846,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -860,6 +860,9 @@
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.1.csv</v>
@@ -872,6 +875,9 @@
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.2.csv</v>
@@ -882,7 +888,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -894,7 +903,10 @@
         <v>8.4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -906,7 +918,10 @@
         <v>8.5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -918,7 +933,10 @@
         <v>8.6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -930,7 +948,7 @@
         <v>9.1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -942,7 +960,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -954,7 +972,7 @@
         <v>10.1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
added test files part 3
</commit_message>
<xml_diff>
--- a/testfiles/Tests.xlsx
+++ b/testfiles/Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dumacduke-my.sharepoint.com/personal/dpazzula_dumac_duke_edu/Documents/Documents/FinTech545_Fall2023/testfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67110BD-B845-4D63-BBDC-92D93476919A}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_F25DC773A252ABDACC10488DC99B48205ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20FC16AB-1682-4235-BE05-82D5CA2CFDEB}"/>
   <bookViews>
-    <workbookView xWindow="-25560" yWindow="1560" windowWidth="21735" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22860" yWindow="885" windowWidth="21735" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Test</t>
   </si>
@@ -155,15 +155,6 @@
     <t>ES from T Distribution</t>
   </si>
   <si>
-    <t>Gaussian Copula with a  Normal and T distribution</t>
-  </si>
-  <si>
-    <t>Gaussian Copula with a  2 T distributions</t>
-  </si>
-  <si>
-    <t>VaR/ES on 2 levels from simulated values</t>
-  </si>
-  <si>
     <t>test7_1.csv</t>
   </si>
   <si>
@@ -177,6 +168,12 @@
   </si>
   <si>
     <t>ES from Simulation -- compare to 8.5 values</t>
+  </si>
+  <si>
+    <t>test9_1_portfolio.csv, test9_1_returns.csv</t>
+  </si>
+  <si>
+    <t>VaR/ES on 2 levels from simulated values - Copula</t>
   </si>
 </sst>
 </file>
@@ -497,16 +494,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.5703125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,7 +814,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -831,7 +829,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -846,7 +844,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -861,7 +859,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -876,7 +874,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -888,10 +886,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -906,7 +904,7 @@
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -921,7 +919,7 @@
         <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -933,50 +931,29 @@
         <v>8.6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>testout_8.6.csv</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9.1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>testout_9.1.csv</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>testout_9.2.csv</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>10.1</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>testout_10.1.csv</v>
       </c>
     </row>
   </sheetData>

</xml_diff>